<commit_message>
Working dev build, without login
</commit_message>
<xml_diff>
--- a/flaskr/files/Valuebestand.xlsx
+++ b/flaskr/files/Valuebestand.xlsx
@@ -386,7 +386,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Random data</t>
+          <t>Plaats om de data te plaatsen yeet</t>
         </is>
       </c>
     </row>
@@ -401,11 +401,6 @@
           <t>K12 uit Mergebestand oeet1</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>K12 uit Mergebestand leet3</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -418,11 +413,6 @@
           <t>K23 uit Mergebestand reet2</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>K23 uit Mergebestand yeet1</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -435,11 +425,6 @@
           <t>K34 uit Mergebestand weet3</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>K34 uit Mergebestand heet5</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -452,11 +437,6 @@
           <t>K45 uit Mergebestand qeet4</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>K45 uit Mergebestand neet2</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -467,11 +447,6 @@
       <c r="B6" t="inlineStr">
         <is>
           <t>K56 uit Mergebestand meet5</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>K56 uit Mergebestand keet4</t>
         </is>
       </c>
     </row>

</xml_diff>